<commit_message>
Day 3 Framework changes
</commit_message>
<xml_diff>
--- a/data/TC02.xlsx
+++ b/data/TC02.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>UserName</t>
   </si>
@@ -25,18 +25,6 @@
   </si>
   <si>
     <t>mathan@credosystemz.sanbox</t>
-  </si>
-  <si>
-    <t>lastName</t>
-  </si>
-  <si>
-    <t>companyName</t>
-  </si>
-  <si>
-    <t>Raja</t>
-  </si>
-  <si>
-    <t>Credo Learning</t>
   </si>
   <si>
     <t>Mylearning$2</t>
@@ -389,45 +377,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>